<commit_message>
modified:   Data Augmentation.ipynb 	modified:   Food Wasteage Data.xlsx 	new file:   augmented.csv 	modified:   foodwastage.csv
</commit_message>
<xml_diff>
--- a/Food Wasteage Data.xlsx
+++ b/Food Wasteage Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrshv\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrshv\Documents\Corrected-Speech-to-Text-with-BERT-and-Wav2Vec2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4DD921-3FAA-427F-B7F8-389EB5D3D396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E2F875-EC8F-4A6B-A61A-0E6286882CB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{C7317C44-D9AF-47A8-A86E-0B8C3D3026E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{C7317C44-D9AF-47A8-A86E-0B8C3D3026E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBECD10-CEFF-4C81-B7E2-DE3345A62CA7}">
   <dimension ref="A1:AL18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2240,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CB9E76-338A-4316-9EA2-877851F12A85}">
   <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:S1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>